<commit_message>
<< 칼럼 삭제>>  "태그리스트: 21-06" * TBL_CONTROL_PART   - MATERIAL_FINISH_TM   - UNIT_MATERIAL_FINISH_TM_AUTO_AMT   - UNIT_MATERIAL_FINISH_TM_AMT
* TBL_ESTIMATE_DETAIL
  - MATERIAL_FINISH_TM
  - UNIT_MATERIAL_FINISH_TM_AUTO_AMT
  - UNIT_MATERIAL_FINISH_TM_AMT
</commit_message>
<xml_diff>
--- a/src/main/resources/excelTemplate/estimate_list_template.xlsx
+++ b/src/main/resources/excelTemplate/estimate_list_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>규격</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -103,10 +103,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>각비</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>포
 켓</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -217,18 +213,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${data.MATERIAL_DETAIL_NM}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${data.SURFACE_TREAT_NM}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${data.MATERIAL_FINISH_GRIND_NM}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>${data.PART_NUM}//:1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -280,11 +264,19 @@
     <t>${data.ROWNUM}//:1</t>
   </si>
   <si>
-    <t>${data.UNIT_MATERIAL_FINISH_TM_AMT}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${data.UNIT_MATERIAL_FINISH_HEAT_AMT}</t>
+    <t>${data.MATERIAL_DETAIL_NM}//:1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.SURFACE_TREAT_NM}//:1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.MATERIAL_FINISH_GRIND_NM}//:1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${data.UNIT_MATERIAL_FINISH_HEAT_AMT}//:1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -292,9 +284,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -401,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -527,6 +518,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -536,113 +566,110 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="41" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="41" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -707,8 +734,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6324600" y="552450"/>
-          <a:ext cx="2752725" cy="8394456"/>
+          <a:off x="6315075" y="552450"/>
+          <a:ext cx="2676525" cy="8394456"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1004,247 +1031,246 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="5.125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="4.25" style="8" customWidth="1"/>
-    <col min="7" max="7" width="5" style="8" customWidth="1"/>
-    <col min="8" max="8" width="8.125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="8.75" style="8" customWidth="1"/>
-    <col min="10" max="10" width="7.375" style="8" customWidth="1"/>
-    <col min="11" max="11" width="7.25" style="8" customWidth="1"/>
-    <col min="12" max="19" width="4.375" style="8" customWidth="1"/>
-    <col min="20" max="21" width="8.375" style="8" customWidth="1"/>
-    <col min="22" max="22" width="10.375" style="8" customWidth="1"/>
-    <col min="23" max="23" width="9" style="8" customWidth="1"/>
-    <col min="24" max="24" width="10.25" style="8" customWidth="1"/>
-    <col min="25" max="25" width="8.375" style="8" customWidth="1"/>
-    <col min="26" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="3.125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="3.125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="5.125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="4.25" style="6" customWidth="1"/>
+    <col min="7" max="7" width="5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.75" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.25" style="6" customWidth="1"/>
+    <col min="12" max="19" width="4.375" style="6" customWidth="1"/>
+    <col min="20" max="21" width="8.375" style="6" customWidth="1"/>
+    <col min="22" max="22" width="10.375" style="6" customWidth="1"/>
+    <col min="23" max="23" width="9" style="6" customWidth="1"/>
+    <col min="24" max="24" width="10.25" style="6" customWidth="1"/>
+    <col min="25" max="25" width="8.375" style="6" customWidth="1"/>
+    <col min="26" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="23" t="s">
+      <c r="K1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="15" t="s">
+      <c r="R1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+      <c r="V1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" s="29" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="18" t="s">
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="P2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="30"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="17"/>
     </row>
     <row r="3" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="U3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="V3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="25" t="s">
+      <c r="W3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="V3" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y3" s="34" t="s">
-        <v>48</v>
+      <c r="Y3" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
+  <mergeCells count="37">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="X1:X2"/>
     <mergeCell ref="Y1:Y2"/>
@@ -1261,15 +1287,17 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>